<commit_message>
Updated an neue cleaned
</commit_message>
<xml_diff>
--- a/felix_playground_SQA_Training/module_guide_sqa_contents.xlsx
+++ b/felix_playground_SQA_Training/module_guide_sqa_contents.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="349">
   <si>
     <t>id</t>
   </si>
@@ -43,91 +43,91 @@
     <t xml:space="preserve">Give me the content of the module Information Processing within Organizations? </t>
   </si>
   <si>
-    <t>What is the content of IT-Management?</t>
+    <t>Give me the content of IT-Management?</t>
   </si>
   <si>
     <t>Give me the content of Project Seminar?</t>
   </si>
   <si>
-    <t>What is the content of Information Retrieval?</t>
+    <t>What is the description of Information Retrieval?</t>
   </si>
   <si>
     <t>What is the content of Analysis and Design of Programs?</t>
   </si>
   <si>
-    <t>What is the content of Security of Software Systems?</t>
-  </si>
-  <si>
-    <t>What is the description of Software Architecture?</t>
-  </si>
-  <si>
-    <t>What is Artificial Intelligence 1 about?</t>
+    <t xml:space="preserve">Give me the content of the module Security of Software Systems? </t>
+  </si>
+  <si>
+    <t>What is Software Architecture about?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Artificial Intelligence 1? </t>
   </si>
   <si>
     <t>What is the content of Discrete Event Simulation?</t>
   </si>
   <si>
-    <t>What is the content of Advanced Programming?</t>
+    <t xml:space="preserve">Give me the content of the module Advanced Programming? </t>
   </si>
   <si>
     <t>What is the content of Programming with neural nets?</t>
   </si>
   <si>
-    <t>What is the content of NLP and Text Mining?</t>
-  </si>
-  <si>
-    <t>What is the content of Systems Benchmarking?</t>
+    <t xml:space="preserve">Give me the content of the module NLP and Text Mining? </t>
+  </si>
+  <si>
+    <t>What is Systems Benchmarking about?</t>
   </si>
   <si>
     <t>Give me the content of Computer Vision?</t>
   </si>
   <si>
-    <t>What is the description of Image Processing and Computational Photography?</t>
-  </si>
-  <si>
-    <t>What is Multilingual NLP about?</t>
-  </si>
-  <si>
-    <t>Give me the content of Statistical Network Analysis?</t>
-  </si>
-  <si>
-    <t>What is the description of Operations Research?</t>
-  </si>
-  <si>
-    <t>What is Machine Learning for Networks 1 about?</t>
-  </si>
-  <si>
-    <t>What is the description of Data Science?</t>
+    <t>What is Image Processing and Computational Photography about?</t>
+  </si>
+  <si>
+    <t>What is the content of Multilingual NLP?</t>
+  </si>
+  <si>
+    <t>What is the content of Statistical Network Analysis?</t>
+  </si>
+  <si>
+    <t>What is the content of Operations Research?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Machine Learning for Networks 1? </t>
+  </si>
+  <si>
+    <t>Give me the content of Data Science?</t>
   </si>
   <si>
     <t>What is the description of Business Software 1: IS-based Enterprise Management?</t>
   </si>
   <si>
-    <t xml:space="preserve">Give me the content of the module Business Software 2: Enterprise Resource Planning Systems? </t>
-  </si>
-  <si>
-    <t>What is Advanced Seminar: Enterprise Systems about?</t>
-  </si>
-  <si>
-    <t>What is the content of Decision Support Systems?</t>
-  </si>
-  <si>
-    <t>Give me the content of Analytical Information Systems?</t>
-  </si>
-  <si>
-    <t>What is Business Analytics about?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module E-Business Strategies? </t>
+    <t>What is the content of Business Software 2: Enterprise Resource Planning Systems?</t>
+  </si>
+  <si>
+    <t>Give me the content of Advanced Seminar: Enterprise Systems?</t>
+  </si>
+  <si>
+    <t>What is the description of Decision Support Systems?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Analytical Information Systems? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Business Analytics? </t>
+  </si>
+  <si>
+    <t>Give me the content of E-Business Strategies?</t>
   </si>
   <si>
     <t>What is the description of Mobile and Ubiquitous Systems?</t>
   </si>
   <si>
-    <t>What is the description of Seminar: E-Business Strategies?</t>
-  </si>
-  <si>
-    <t>What is the description of Corporate Entrepreneurship?</t>
+    <t xml:space="preserve">Give me the content of the module Seminar: E-Business Strategies? </t>
+  </si>
+  <si>
+    <t>What is Corporate Entrepreneurship about?</t>
   </si>
   <si>
     <t>What is the description of Digital Entrepreneurship?</t>
@@ -139,181 +139,154 @@
     <t>Give me the content of Global Logistics &amp; Supply Chain Management?</t>
   </si>
   <si>
-    <t>Give me the content of Advanced Operations &amp; Logistics Management?</t>
-  </si>
-  <si>
-    <t>What is the content of Seminar: Operations Management?</t>
-  </si>
-  <si>
-    <t>Give me the content of Adaption and Continuous System Engineering?</t>
-  </si>
-  <si>
-    <t>Give me the content of Business Service Platforms 2?</t>
-  </si>
-  <si>
-    <t>Give me the content of Business Service Platforms 1?</t>
-  </si>
-  <si>
-    <t>Give me the content of Abbreviation?</t>
+    <t>What is the description of Advanced Operations &amp; Logistics Management?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Seminar: Operations Management? </t>
+  </si>
+  <si>
+    <t>What is Adaption and Continuous System Engineering about?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Business Service Platforms 2? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Business Service Platforms 1? </t>
+  </si>
+  <si>
+    <t>What is Abbreviation about?</t>
   </si>
   <si>
     <t>What is Work and Information about?</t>
   </si>
   <si>
-    <t>What is Work Order Planning for Automated Manufacturing about?</t>
+    <t>Give me the content of Work Order Planning for Automated Manufacturing?</t>
   </si>
   <si>
     <t>Give me the content of Topics in Business Information Systems 1?</t>
   </si>
   <si>
-    <t>Give me the content of Topics in Business Information Systems 2?</t>
-  </si>
-  <si>
-    <t>What is the description of Information systems research?</t>
-  </si>
-  <si>
-    <t>What is the description of Databases 2?</t>
+    <t>What is Topics in Business Information Systems 2 about?</t>
+  </si>
+  <si>
+    <t>Give me the content of Information systems research?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Databases 2? </t>
   </si>
   <si>
     <t>What is the description of Compiler Construction?</t>
   </si>
   <si>
-    <t>What is Information Retrieval about?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Artificial Intelligence 1? </t>
-  </si>
-  <si>
-    <t>Give me the content of Artificial Intelligence 2?</t>
-  </si>
-  <si>
-    <t>What is the description of E-Learning?</t>
-  </si>
-  <si>
-    <t>What is Analysis and Design of Programs about?</t>
-  </si>
-  <si>
-    <t>What is Professional Project Management about?</t>
-  </si>
-  <si>
-    <t>What is the description of Algorithms for Geographic Information Systems?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Real-Time Interactive Systems? </t>
-  </si>
-  <si>
-    <t>Give me the content of Logic Programming?</t>
-  </si>
-  <si>
-    <t>What is the content of Machine Learning for Natural Language Processing?</t>
-  </si>
-  <si>
-    <t>Give me the content of Medical Informatics?</t>
-  </si>
-  <si>
-    <t>What is Performance Engineering &amp; Benchmarking of Computer Systems about?</t>
-  </si>
-  <si>
-    <t>Give me the content of Programming with neural nets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Robotics 1? </t>
-  </si>
-  <si>
-    <t>What is the description of Security of Software Systems?</t>
-  </si>
-  <si>
-    <t>Give me the content of Discrete Event Simulation?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Software Architecture? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module NLP and Text Mining? </t>
-  </si>
-  <si>
-    <t>What is the description of Project - Current Topics in Computer Science?</t>
+    <t>What is Artificial Intelligence 2 about?</t>
+  </si>
+  <si>
+    <t>Give me the content of E-Learning?</t>
+  </si>
+  <si>
+    <t>Give me the content of Professional Project Management?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Algorithms for Geographic Information Systems? </t>
+  </si>
+  <si>
+    <t>What is the content of Real-Time Interactive Systems?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Logic Programming? </t>
+  </si>
+  <si>
+    <t>Give me the content of Machine Learning for Natural Language Processing?</t>
+  </si>
+  <si>
+    <t>What is Medical Informatics about?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Performance Engineering &amp; Benchmarking of Computer Systems? </t>
+  </si>
+  <si>
+    <t>What is the description of Robotics 1?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Project - Current Topics in Computer Science? </t>
   </si>
   <si>
     <t>What is International Marketing about?</t>
   </si>
   <si>
-    <t xml:space="preserve">Give me the content of the module Brand Management &amp; Market Research? </t>
+    <t>What is the description of Brand Management &amp; Market Research?</t>
   </si>
   <si>
     <t xml:space="preserve">Give me the content of the module Strategic Networks in Industry? </t>
   </si>
   <si>
-    <t>What is the content of Strategic Marketing?</t>
-  </si>
-  <si>
-    <t>What is the description of Industrial Management 4?</t>
-  </si>
-  <si>
-    <t>Give me the content of Industrial Management 2?</t>
+    <t>Give me the content of Strategic Marketing?</t>
+  </si>
+  <si>
+    <t>What is Industrial Management 4 about?</t>
+  </si>
+  <si>
+    <t>What is the description of Industrial Management 2?</t>
   </si>
   <si>
     <t>What is the description of Industrial Management 1?</t>
   </si>
   <si>
-    <t>What is the content of Industrial Management 3?</t>
-  </si>
-  <si>
-    <t>Give me the content of Legal Foundations of Risk Management and Compliance?</t>
-  </si>
-  <si>
-    <t>What is the content of Financial Statement Analysis and Business Valuation?</t>
-  </si>
-  <si>
-    <t>What is the content of Philosophy of Science and Ethics in Business Management and Economics?</t>
-  </si>
-  <si>
-    <t>What is Risk Management - Concepts and Systems about?</t>
-  </si>
-  <si>
-    <t>What is Discounted Cashflow about?</t>
-  </si>
-  <si>
-    <t>What is Portfolio and Capital Market Theory about?</t>
-  </si>
-  <si>
-    <t>What is the description of Risk Management and Corporate Finance?</t>
-  </si>
-  <si>
-    <t>Give me the content of Risk measurement and risk valuation: Concepts and applications for banks?</t>
+    <t>What is the description of Industrial Management 3?</t>
+  </si>
+  <si>
+    <t>What is the description of Legal Foundations of Risk Management and Compliance?</t>
+  </si>
+  <si>
+    <t>What is the description of Financial Statement Analysis and Business Valuation?</t>
+  </si>
+  <si>
+    <t>Give me the content of Philosophy of Science and Ethics in Business Management and Economics?</t>
+  </si>
+  <si>
+    <t>What is the content of Risk Management - Concepts and Systems?</t>
+  </si>
+  <si>
+    <t>What is the description of Discounted Cashflow?</t>
+  </si>
+  <si>
+    <t>What is the content of Portfolio and Capital Market Theory?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Risk Management and Corporate Finance? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Risk measurement and risk valuation: Concepts and applications for banks? </t>
   </si>
   <si>
     <t>Give me the content of Economics of Tax Planning?</t>
   </si>
   <si>
-    <t>What is Tax Accounting about?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Incentives in Organizations? </t>
-  </si>
-  <si>
-    <t>What is Human Resource Management and Industrial Relations about?</t>
-  </si>
-  <si>
-    <t>Give me the content of Advanced Seminar: Entrepreneurship and Management?</t>
-  </si>
-  <si>
-    <t>What is the content of Corporate Strategy?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Change Management? </t>
-  </si>
-  <si>
-    <t>What is Managerial Accounting in the Company Management about?</t>
-  </si>
-  <si>
-    <t>What is the description of Strategic Managerial Accounting?</t>
-  </si>
-  <si>
-    <t>Give me the content of Coordination, Budgeting and Incentives in Organizations?</t>
-  </si>
-  <si>
-    <t>What is the content of Project Management and Control?</t>
+    <t>What is the content of Tax Accounting?</t>
+  </si>
+  <si>
+    <t>What is the content of Incentives in Organizations?</t>
+  </si>
+  <si>
+    <t>Give me the content of Human Resource Management and Industrial Relations?</t>
+  </si>
+  <si>
+    <t>Give me the content of Corporate Strategy?</t>
+  </si>
+  <si>
+    <t>What is the description of Change Management?</t>
+  </si>
+  <si>
+    <t>Give me the content of Managerial Accounting in the Company Management?</t>
+  </si>
+  <si>
+    <t>What is the content of Strategic Managerial Accounting?</t>
+  </si>
+  <si>
+    <t>What is Coordination, Budgeting and Incentives in Organizations about?</t>
+  </si>
+  <si>
+    <t>What is the description of Project Management and Control?</t>
   </si>
   <si>
     <t>Give me the content of Accounting and Capital Markets?</t>
@@ -322,91 +295,91 @@
     <t>What is Managerial Analytics &amp; Decision Making about?</t>
   </si>
   <si>
-    <t>What is the description of Strategic Management of Global Supply Chains?</t>
-  </si>
-  <si>
-    <t>Give me the content of Strategic Decisions and Competition?</t>
-  </si>
-  <si>
-    <t>What is Theory of Industrial Organization about?</t>
-  </si>
-  <si>
-    <t>What is the content of European Competition Policy?</t>
-  </si>
-  <si>
-    <t>What is the description of Econometrics 1?</t>
-  </si>
-  <si>
-    <t>What is Advanced Microeconomics about?</t>
-  </si>
-  <si>
-    <t>What is the description of Selected Topics in Business Management and Economics 1?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Selected Topics in Business Management and Economics 2? </t>
-  </si>
-  <si>
-    <t>Give me the content of Selected Topics in Business Information Systems 1?</t>
-  </si>
-  <si>
-    <t>What is the content of Selected Topics in Business Information Systems 2?</t>
+    <t>What is the content of Strategic Management of Global Supply Chains?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Strategic Decisions and Competition? </t>
+  </si>
+  <si>
+    <t>What is the content of Theory of Industrial Organization?</t>
+  </si>
+  <si>
+    <t>What is the description of European Competition Policy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Econometrics 1? </t>
+  </si>
+  <si>
+    <t>What is the content of Advanced Microeconomics?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Selected Topics in Business Management and Economics 1? </t>
+  </si>
+  <si>
+    <t>What is Selected Topics in Business Management and Economics 2 about?</t>
+  </si>
+  <si>
+    <t>What is the description of Selected Topics in Business Information Systems 1?</t>
+  </si>
+  <si>
+    <t>What is the description of Selected Topics in Business Information Systems 2?</t>
   </si>
   <si>
     <t>What is the content of Digital Marketing I?</t>
   </si>
   <si>
-    <t xml:space="preserve">Give me the content of the module Digital Marketing II? </t>
-  </si>
-  <si>
-    <t>Give me the content of E-Commerce I?</t>
-  </si>
-  <si>
-    <t>Give me the content of E-Commerce II?</t>
-  </si>
-  <si>
-    <t>What is Real-Time Process Analytics about?</t>
-  </si>
-  <si>
-    <t>What is Topics in Data Science about?</t>
-  </si>
-  <si>
-    <t>What is Topics in Information Systems 1 about?</t>
-  </si>
-  <si>
-    <t>What is the description of Topics in Information Systems 2?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Stochastic Models for Risk Analysis? </t>
-  </si>
-  <si>
-    <t>What is the description of Stochastic Models for Risk Assessment?</t>
+    <t>What is the content of Digital Marketing II?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module E-Commerce I? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module E-Commerce II? </t>
+  </si>
+  <si>
+    <t>What is the content of Real-Time Process Analytics?</t>
+  </si>
+  <si>
+    <t>Give me the content of Topics in Data Science?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module Topics in Information Systems 1? </t>
+  </si>
+  <si>
+    <t>What is the content of Topics in Information Systems 2?</t>
+  </si>
+  <si>
+    <t>What is Stochastic Models for Risk Analysis about?</t>
+  </si>
+  <si>
+    <t>What is Stochastic Models for Risk Assessment about?</t>
   </si>
   <si>
     <t xml:space="preserve">Give me the content of the module Communication in Business and Economics? </t>
   </si>
   <si>
-    <t xml:space="preserve">Give me the content of the module Business Communication in Print, Online and Social Media? </t>
-  </si>
-  <si>
-    <t>What is the content of Managerial Practice Lectures?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Advanced Topics in Data Science? </t>
-  </si>
-  <si>
-    <t>What is International Marketing Strategy about?</t>
+    <t>What is the content of Business Communication in Print, Online and Social Media?</t>
+  </si>
+  <si>
+    <t>Give me the content of Managerial Practice Lectures?</t>
+  </si>
+  <si>
+    <t>What is the content of Advanced Topics in Data Science?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me the content of the module International Marketing Strategy? </t>
   </si>
   <si>
     <t>What is the content of Economist Practice Lectures?</t>
   </si>
   <si>
-    <t>What is Enterprise AI about?</t>
-  </si>
-  <si>
-    <t>What is Information Systems and Artificial Intelligence 1 about?</t>
-  </si>
-  <si>
-    <t>What is the content of Information Systems and Artificial Intelligence 2?</t>
+    <t>Give me the content of Enterprise AI?</t>
+  </si>
+  <si>
+    <t>What is the description of Information Systems and Artificial Intelligence 1?</t>
+  </si>
+  <si>
+    <t>Give me the content of Information Systems and Artificial Intelligence 2?</t>
   </si>
   <si>
     <t>Give me the content of Vertical Storytelling?</t>
@@ -418,25 +391,7 @@
     <t>Give me the content of Policy Evaluation Methods?</t>
   </si>
   <si>
-    <t>What is the description of Topics in Empirical Economics?</t>
-  </si>
-  <si>
-    <t>What is the description of Systems Benchmarking?</t>
-  </si>
-  <si>
-    <t>What is Computer Vision about?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give me the content of the module Image Processing and Computational Photography? </t>
-  </si>
-  <si>
-    <t>What is the content of Multilingual NLP?</t>
-  </si>
-  <si>
-    <t>What is Operations Research about?</t>
-  </si>
-  <si>
-    <t>What is Data Science about?</t>
+    <t>Give me the content of Topics in Empirical Economics?</t>
   </si>
   <si>
     <t>What is Master Thesis Information Systems about?</t>
@@ -803,54 +758,6 @@
   </si>
   <si>
     <t>['(119, 8)']</t>
-  </si>
-  <si>
-    <t>['(120, 8)']</t>
-  </si>
-  <si>
-    <t>['(121, 8)']</t>
-  </si>
-  <si>
-    <t>['(122, 8)']</t>
-  </si>
-  <si>
-    <t>['(123, 8)']</t>
-  </si>
-  <si>
-    <t>['(124, 8)']</t>
-  </si>
-  <si>
-    <t>['(125, 8)']</t>
-  </si>
-  <si>
-    <t>['(126, 8)']</t>
-  </si>
-  <si>
-    <t>['(127, 8)']</t>
-  </si>
-  <si>
-    <t>['(128, 8)']</t>
-  </si>
-  <si>
-    <t>['(129, 8)']</t>
-  </si>
-  <si>
-    <t>['(130, 8)']</t>
-  </si>
-  <si>
-    <t>['(131, 8)']</t>
-  </si>
-  <si>
-    <t>['(132, 8)']</t>
-  </si>
-  <si>
-    <t>['(133, 8)']</t>
-  </si>
-  <si>
-    <t>['(134, 8)']</t>
-  </si>
-  <si>
-    <t>['(135, 8)']</t>
   </si>
   <si>
     <t>['Content:
@@ -2177,7 +2084,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2220,13 +2127,13 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2243,13 +2150,13 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2266,13 +2173,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2289,13 +2196,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2312,13 +2219,13 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2335,13 +2242,13 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2358,13 +2265,13 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2381,13 +2288,13 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2404,13 +2311,13 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="G10" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2427,13 +2334,13 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="G11" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2450,13 +2357,13 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="G12" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2473,13 +2380,13 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F13" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="G13" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2496,13 +2403,13 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="G14" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2519,13 +2426,13 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="G15" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2542,13 +2449,13 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" t="s">
         <v>142</v>
       </c>
-      <c r="F16" t="s">
-        <v>157</v>
-      </c>
       <c r="G16" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2565,13 +2472,13 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="G17" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2588,13 +2495,13 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="G18" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2611,13 +2518,13 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="G19" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2634,13 +2541,13 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="G20" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2657,13 +2564,13 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="G21" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2680,13 +2587,13 @@
         <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="G22" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2703,13 +2610,13 @@
         <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="G23" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2726,13 +2633,13 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="G24" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2749,13 +2656,13 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F25" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="G25" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2772,13 +2679,13 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F26" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="G26" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2795,13 +2702,13 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="G27" t="s">
-        <v>300</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2818,13 +2725,13 @@
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F28" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="G28" t="s">
-        <v>301</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2841,13 +2748,13 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F29" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="G29" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2864,13 +2771,13 @@
         <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F30" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="G30" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2887,13 +2794,13 @@
         <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F31" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="G31" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2910,13 +2817,13 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="G32" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2933,13 +2840,13 @@
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F33" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="G33" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2956,13 +2863,13 @@
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F34" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="G34" t="s">
-        <v>307</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2979,13 +2886,13 @@
         <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F35" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G35" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3002,13 +2909,13 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="G36" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3025,13 +2932,13 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F37" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="G37" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3048,13 +2955,13 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F38" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="G38" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3071,13 +2978,13 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="G39" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3094,13 +3001,13 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F40" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="G40" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3117,13 +3024,13 @@
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="G41" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3140,13 +3047,13 @@
         <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F42" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="G42" t="s">
-        <v>315</v>
+        <v>284</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3163,13 +3070,13 @@
         <v>49</v>
       </c>
       <c r="E43" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="G43" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3186,13 +3093,13 @@
         <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F44" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="G44" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3209,13 +3116,13 @@
         <v>51</v>
       </c>
       <c r="E45" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F45" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="G45" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3232,13 +3139,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F46" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G46" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3255,13 +3162,13 @@
         <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="G47" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3278,13 +3185,13 @@
         <v>54</v>
       </c>
       <c r="E48" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F48" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="G48" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3301,13 +3208,13 @@
         <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F49" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G49" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3324,13 +3231,13 @@
         <v>56</v>
       </c>
       <c r="E50" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F50" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="G50" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3347,13 +3254,13 @@
         <v>57</v>
       </c>
       <c r="E51" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F51" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="G51" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3370,13 +3277,13 @@
         <v>58</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F52" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G52" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3393,13 +3300,13 @@
         <v>59</v>
       </c>
       <c r="E53" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F53" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="G53" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3416,13 +3323,13 @@
         <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F54" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G54" t="s">
-        <v>323</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3439,13 +3346,13 @@
         <v>61</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F55" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G55" t="s">
-        <v>324</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3462,13 +3369,13 @@
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F56" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="G56" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3482,16 +3389,16 @@
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F57" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G57" t="s">
-        <v>326</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3505,16 +3412,16 @@
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E58" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F58" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="G58" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3528,16 +3435,16 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F59" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="G59" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3551,16 +3458,16 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F60" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G60" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3574,16 +3481,16 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F61" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G61" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3597,16 +3504,16 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F62" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G62" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3620,16 +3527,16 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F63" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="G63" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3643,16 +3550,16 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E64" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F64" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="G64" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3666,16 +3573,16 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F65" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G65" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3689,16 +3596,16 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E66" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F66" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G66" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3712,16 +3619,16 @@
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F67" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="G67" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3735,16 +3642,16 @@
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E68" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F68" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="G68" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3758,16 +3665,16 @@
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E69" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F69" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="G69" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3781,16 +3688,16 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F70" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="G70" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3804,16 +3711,16 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F71" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G71" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3827,16 +3734,16 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E72" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F72" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G72" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3850,16 +3757,16 @@
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E73" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F73" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="G73" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3873,16 +3780,16 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F74" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G74" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3896,16 +3803,16 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F75" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="G75" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3919,16 +3826,16 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F76" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="G76" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3942,16 +3849,16 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E77" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F77" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="G77" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3965,16 +3872,16 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F78" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="G78" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3988,16 +3895,16 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E79" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F79" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="G79" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4011,16 +3918,16 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E80" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F80" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="G80" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4034,16 +3941,16 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F81" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="G81" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4057,16 +3964,16 @@
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F82" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G82" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4080,16 +3987,16 @@
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E83" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F83" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="G83" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4103,16 +4010,16 @@
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F84" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="G84" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4126,16 +4033,16 @@
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E85" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F85" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="G85" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4149,16 +4056,16 @@
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E86" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F86" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="G86" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4172,16 +4079,16 @@
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E87" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F87" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="G87" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4195,16 +4102,16 @@
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E88" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F88" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G88" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4218,16 +4125,16 @@
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E89" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F89" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="G89" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4241,16 +4148,16 @@
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E90" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F90" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G90" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4264,16 +4171,16 @@
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E91" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F91" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="G91" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4287,16 +4194,16 @@
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E92" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F92" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="G92" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4310,16 +4217,16 @@
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E93" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F93" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="G93" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4333,16 +4240,16 @@
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E94" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F94" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="G94" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4356,16 +4263,16 @@
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E95" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F95" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="G95" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4379,16 +4286,16 @@
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E96" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F96" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="G96" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -4402,16 +4309,16 @@
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E97" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F97" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="G97" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -4425,16 +4332,16 @@
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E98" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F98" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="G98" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -4448,16 +4355,16 @@
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E99" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F99" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G99" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -4471,16 +4378,16 @@
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E100" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F100" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="G100" t="s">
-        <v>362</v>
+        <v>336</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -4494,16 +4401,16 @@
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E101" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F101" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G101" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -4517,16 +4424,16 @@
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E102" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F102" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G102" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4540,16 +4447,16 @@
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E103" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F103" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="G103" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -4563,16 +4470,16 @@
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E104" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F104" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G104" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4586,16 +4493,16 @@
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E105" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F105" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="G105" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4609,16 +4516,16 @@
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E106" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F106" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G106" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -4632,16 +4539,16 @@
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E107" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F107" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="G107" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4655,16 +4562,16 @@
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E108" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F108" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="G108" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4678,16 +4585,16 @@
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E109" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F109" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G109" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -4701,16 +4608,16 @@
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E110" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F110" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="G110" t="s">
-        <v>368</v>
+        <v>343</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4724,16 +4631,16 @@
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E111" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F111" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G111" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4747,16 +4654,16 @@
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E112" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F112" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G112" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4770,16 +4677,16 @@
         <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E113" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F113" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G113" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4793,16 +4700,16 @@
         <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E114" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F114" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G114" t="s">
-        <v>370</v>
+        <v>260</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -4816,16 +4723,16 @@
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E115" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F115" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="G115" t="s">
-        <v>371</v>
+        <v>260</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -4839,16 +4746,16 @@
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E116" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F116" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="G116" t="s">
-        <v>372</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -4862,16 +4769,16 @@
         <v>0</v>
       </c>
       <c r="D117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E117" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F117" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="G117" t="s">
-        <v>373</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4885,16 +4792,16 @@
         <v>0</v>
       </c>
       <c r="D118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E118" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F118" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="G118" t="s">
-        <v>374</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -4908,16 +4815,16 @@
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E119" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F119" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G119" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -4931,16 +4838,16 @@
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E120" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F120" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="G120" t="s">
-        <v>376</v>
+        <v>260</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4954,384 +4861,16 @@
         <v>0</v>
       </c>
       <c r="D121" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E121" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F121" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="G121" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="A122" t="s">
-        <v>7</v>
-      </c>
-      <c r="B122">
-        <v>0</v>
-      </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122" t="s">
-        <v>128</v>
-      </c>
-      <c r="E122" t="s">
-        <v>142</v>
-      </c>
-      <c r="F122" t="s">
-        <v>263</v>
-      </c>
-      <c r="G122" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
-      <c r="A123" t="s">
-        <v>7</v>
-      </c>
-      <c r="B123">
-        <v>0</v>
-      </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-      <c r="D123" t="s">
-        <v>129</v>
-      </c>
-      <c r="E123" t="s">
-        <v>142</v>
-      </c>
-      <c r="F123" t="s">
-        <v>264</v>
-      </c>
-      <c r="G123" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="A124" t="s">
-        <v>7</v>
-      </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-      <c r="D124" t="s">
-        <v>130</v>
-      </c>
-      <c r="E124" t="s">
-        <v>142</v>
-      </c>
-      <c r="F124" t="s">
-        <v>265</v>
-      </c>
-      <c r="G124" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c r="A125" t="s">
-        <v>7</v>
-      </c>
-      <c r="B125">
-        <v>0</v>
-      </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-      <c r="D125" t="s">
-        <v>131</v>
-      </c>
-      <c r="E125" t="s">
-        <v>142</v>
-      </c>
-      <c r="F125" t="s">
-        <v>266</v>
-      </c>
-      <c r="G125" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="A126" t="s">
-        <v>7</v>
-      </c>
-      <c r="B126">
-        <v>0</v>
-      </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-      <c r="D126" t="s">
-        <v>132</v>
-      </c>
-      <c r="E126" t="s">
-        <v>142</v>
-      </c>
-      <c r="F126" t="s">
-        <v>267</v>
-      </c>
-      <c r="G126" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" t="s">
-        <v>7</v>
-      </c>
-      <c r="B127">
-        <v>0</v>
-      </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-      <c r="D127" t="s">
-        <v>133</v>
-      </c>
-      <c r="E127" t="s">
-        <v>142</v>
-      </c>
-      <c r="F127" t="s">
-        <v>268</v>
-      </c>
-      <c r="G127" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c r="A128" t="s">
-        <v>7</v>
-      </c>
-      <c r="B128">
-        <v>0</v>
-      </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-      <c r="D128" t="s">
-        <v>134</v>
-      </c>
-      <c r="E128" t="s">
-        <v>142</v>
-      </c>
-      <c r="F128" t="s">
-        <v>269</v>
-      </c>
-      <c r="G128" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c r="A129" t="s">
-        <v>7</v>
-      </c>
-      <c r="B129">
-        <v>0</v>
-      </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-      <c r="D129" t="s">
-        <v>135</v>
-      </c>
-      <c r="E129" t="s">
-        <v>142</v>
-      </c>
-      <c r="F129" t="s">
-        <v>270</v>
-      </c>
-      <c r="G129" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c r="A130" t="s">
-        <v>7</v>
-      </c>
-      <c r="B130">
-        <v>0</v>
-      </c>
-      <c r="C130">
-        <v>0</v>
-      </c>
-      <c r="D130" t="s">
-        <v>136</v>
-      </c>
-      <c r="E130" t="s">
-        <v>142</v>
-      </c>
-      <c r="F130" t="s">
-        <v>271</v>
-      </c>
-      <c r="G130" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" t="s">
-        <v>7</v>
-      </c>
-      <c r="B131">
-        <v>0</v>
-      </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-      <c r="D131" t="s">
-        <v>137</v>
-      </c>
-      <c r="E131" t="s">
-        <v>142</v>
-      </c>
-      <c r="F131" t="s">
-        <v>272</v>
-      </c>
-      <c r="G131" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" t="s">
-        <v>7</v>
-      </c>
-      <c r="B132">
-        <v>0</v>
-      </c>
-      <c r="C132">
-        <v>0</v>
-      </c>
-      <c r="D132" t="s">
-        <v>138</v>
-      </c>
-      <c r="E132" t="s">
-        <v>142</v>
-      </c>
-      <c r="F132" t="s">
-        <v>273</v>
-      </c>
-      <c r="G132" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
-      <c r="A133" t="s">
-        <v>7</v>
-      </c>
-      <c r="B133">
-        <v>0</v>
-      </c>
-      <c r="C133">
-        <v>0</v>
-      </c>
-      <c r="D133" t="s">
-        <v>24</v>
-      </c>
-      <c r="E133" t="s">
-        <v>142</v>
-      </c>
-      <c r="F133" t="s">
-        <v>274</v>
-      </c>
-      <c r="G133" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7">
-      <c r="A134" t="s">
-        <v>7</v>
-      </c>
-      <c r="B134">
-        <v>0</v>
-      </c>
-      <c r="C134">
-        <v>0</v>
-      </c>
-      <c r="D134" t="s">
-        <v>139</v>
-      </c>
-      <c r="E134" t="s">
-        <v>142</v>
-      </c>
-      <c r="F134" t="s">
-        <v>275</v>
-      </c>
-      <c r="G134" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" t="s">
-        <v>7</v>
-      </c>
-      <c r="B135">
-        <v>0</v>
-      </c>
-      <c r="C135">
-        <v>0</v>
-      </c>
-      <c r="D135" t="s">
-        <v>26</v>
-      </c>
-      <c r="E135" t="s">
-        <v>142</v>
-      </c>
-      <c r="F135" t="s">
-        <v>276</v>
-      </c>
-      <c r="G135" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7">
-      <c r="A136" t="s">
-        <v>7</v>
-      </c>
-      <c r="B136">
-        <v>0</v>
-      </c>
-      <c r="C136">
-        <v>0</v>
-      </c>
-      <c r="D136" t="s">
-        <v>140</v>
-      </c>
-      <c r="E136" t="s">
-        <v>142</v>
-      </c>
-      <c r="F136" t="s">
-        <v>277</v>
-      </c>
-      <c r="G136" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7">
-      <c r="A137" t="s">
-        <v>7</v>
-      </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-      <c r="D137" t="s">
-        <v>141</v>
-      </c>
-      <c r="E137" t="s">
-        <v>142</v>
-      </c>
-      <c r="F137" t="s">
-        <v>278</v>
-      </c>
-      <c r="G137" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>